<commit_message>
Modified Lista projektow do analizy.xlsx
</commit_message>
<xml_diff>
--- a/Lista projektow do analizy.xlsx
+++ b/Lista projektow do analizy.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
-  <si>
-    <t>Grupa projektów</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Nazwa projektu</t>
   </si>
@@ -33,181 +30,148 @@
     <t>I</t>
   </si>
   <si>
-    <t>rails/rails</t>
-  </si>
-  <si>
-    <t>&gt;100</t>
-  </si>
-  <si>
     <t>II</t>
   </si>
   <si>
-    <t>fog/fog</t>
-  </si>
-  <si>
-    <t>80-60</t>
-  </si>
-  <si>
-    <t>leereilly/swot</t>
-  </si>
-  <si>
-    <t>rapid7/metasploit-framework</t>
-  </si>
-  <si>
-    <t>ruby/www.ruby-lang.org</t>
-  </si>
-  <si>
     <t>III</t>
   </si>
   <si>
-    <t>puppetlabs/puppet</t>
-  </si>
-  <si>
-    <t>60-40</t>
-  </si>
-  <si>
-    <t>spree/spree</t>
-  </si>
-  <si>
-    <t>ManageIQ/manageiq</t>
-  </si>
-  <si>
-    <t>cloudfoundry/cloud_controller_ng</t>
-  </si>
-  <si>
     <t>geoserver/geoserver</t>
   </si>
   <si>
-    <t>mitchellh/vagrant</t>
-  </si>
-  <si>
-    <t>opf/openproject</t>
-  </si>
-  <si>
-    <t>puppetlabs/facter</t>
-  </si>
-  <si>
-    <t>jruby/jruby</t>
-  </si>
-  <si>
     <t>IV</t>
   </si>
   <si>
-    <t>Homebrew/homebrew-science</t>
-  </si>
-  <si>
-    <t>40-20</t>
-  </si>
-  <si>
-    <t>diaspora/diaspora</t>
-  </si>
-  <si>
-    <t>rubinius/rubinius</t>
-  </si>
-  <si>
-    <t>instructure/canvas-lms</t>
-  </si>
-  <si>
     <t>DSpace/DSpace</t>
   </si>
   <si>
-    <t>heroku/heroku</t>
-  </si>
-  <si>
-    <t>progit/progit</t>
-  </si>
-  <si>
-    <t>ruby/ruby</t>
-  </si>
-  <si>
     <t>SpongePowered/SpongeAPI</t>
   </si>
   <si>
-    <t>projecthydra/sufia</t>
-  </si>
-  <si>
     <t>timmolter/XChange</t>
   </si>
   <si>
     <t>caelum/vraptor4</t>
   </si>
   <si>
-    <t>Shopify/active_shipping</t>
-  </si>
-  <si>
-    <t>openSUSE/open-build-service</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
     <t>mozilla/MozStumbler</t>
   </si>
   <si>
-    <t>20-0</t>
-  </si>
-  <si>
-    <t>rspec/rspec-core</t>
-  </si>
-  <si>
     <t>BuildCraft/BuildCraft</t>
   </si>
   <si>
-    <t>SpoutDev/Spout</t>
-  </si>
-  <si>
-    <t>alexreisner/geocoder</t>
-  </si>
-  <si>
-    <t>square/okhttp</t>
-  </si>
-  <si>
-    <t>Shopify/shipit-engine</t>
-  </si>
-  <si>
-    <t>puppetlabs/puppetlabs-firewall</t>
-  </si>
-  <si>
     <t>Jasig/cas</t>
   </si>
   <si>
-    <t>jcabi/jcabi-github</t>
-  </si>
-  <si>
-    <t>MarkUsProject/Markus</t>
-  </si>
-  <si>
-    <t>johnbellone/consul-cookbook</t>
-  </si>
-  <si>
     <t>JakeWharton/u2020</t>
   </si>
   <si>
-    <t>hw-cookbooks/graphite</t>
-  </si>
-  <si>
-    <t>Compass/compass-rails</t>
-  </si>
-  <si>
-    <t>celluloid/dcell</t>
-  </si>
-  <si>
-    <t>Albacore/albacore</t>
-  </si>
-  <si>
-    <t>MagLev/maglev</t>
-  </si>
-  <si>
     <t>ActiveJpa/activejpa</t>
   </si>
   <si>
-    <t>dejan/auto_html</t>
-  </si>
-  <si>
     <t>AzureAD/azure-activedirectory-library-for-android</t>
   </si>
   <si>
-    <t>pawurb/termit</t>
+    <t>java</t>
+  </si>
+  <si>
+    <t>gradle/gradle</t>
+  </si>
+  <si>
+    <t>broadinstitute/picard</t>
+  </si>
+  <si>
+    <t>google/bazel</t>
+  </si>
+  <si>
+    <t>dropwizard/dropwizard</t>
+  </si>
+  <si>
+    <t>google/closure-compiler</t>
+  </si>
+  <si>
+    <t>SpongePowered/Sponge</t>
+  </si>
+  <si>
+    <t>bitcoinj/bitcoinj</t>
+  </si>
+  <si>
+    <t>igniterealtime/Openfire</t>
+  </si>
+  <si>
+    <t>HubSpot/Singularity</t>
+  </si>
+  <si>
+    <t>bndtools/bnd</t>
+  </si>
+  <si>
+    <t>facebook/presto</t>
+  </si>
+  <si>
+    <t>GoogleCloudPlatform/DataflowJavaSDK</t>
+  </si>
+  <si>
+    <t>ReactiveX/RxJava</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>CloudifySource/cloudify</t>
+  </si>
+  <si>
+    <t>L2J/L2J_Server</t>
+  </si>
+  <si>
+    <t>Berico-Technologies/CLAVIN</t>
+  </si>
+  <si>
+    <t>BaseXdb/basex</t>
+  </si>
+  <si>
+    <t>CyberAgent/android-gpuimage</t>
+  </si>
+  <si>
+    <t>47deg/appsly-android-rest</t>
+  </si>
+  <si>
+    <t>Lp.</t>
+  </si>
+  <si>
+    <t>Grupa</t>
+  </si>
+  <si>
+    <t>403 projekty javowe ogółem, wybrano 30</t>
+  </si>
+  <si>
+    <t>język</t>
+  </si>
+  <si>
+    <t>&gt;30</t>
+  </si>
+  <si>
+    <t>25-30</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>10-14</t>
+  </si>
+  <si>
+    <t>5-9</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>1-4</t>
   </si>
 </sst>
 </file>
@@ -368,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +510,48 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -709,8 +715,48 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,6 +940,38 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
@@ -955,54 +1033,66 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Lista projektow do analizy'!$D$2:$D$3,'Lista projektow do analizy'!$D$7,'Lista projektow do analizy'!$D$16,'Lista projektow do analizy'!$D$30)</c:f>
+              <c:f>('Lista projektow do analizy'!$F$3,'Lista projektow do analizy'!$F$6,'Lista projektow do analizy'!$F$10,'Lista projektow do analizy'!$F$15,'Lista projektow do analizy'!$F$19,'Lista projektow do analizy'!$F$24,'Lista projektow do analizy'!$F$29)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>&gt;100</c:v>
+                  <c:v>&gt;30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80-60</c:v>
+                  <c:v>25-30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60-40</c:v>
+                  <c:v>20-24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40-20</c:v>
+                  <c:v>15-19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20-0</c:v>
+                  <c:v>10-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1-4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Lista projektow do analizy'!$E$2:$E$3,'Lista projektow do analizy'!$E$7,'Lista projektow do analizy'!$E$16,'Lista projektow do analizy'!$E$30)</c:f>
+              <c:f>('Lista projektow do analizy'!$G$3,'Lista projektow do analizy'!$G$6,'Lista projektow do analizy'!$G$10,'Lista projektow do analizy'!$G$15,'Lista projektow do analizy'!$G$19,'Lista projektow do analizy'!$G$24,'Lista projektow do analizy'!$G$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2E8F-4BCF-B855-823EC238F134}"/>
+              <c16:uniqueId val="{00000000-4240-49B9-8EA6-EB91A3BF57D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1656,20 +1746,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1984,477 +2074,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="F29" activeCellId="6" sqref="F3:G3 F6:G6 F10:G10 F15:G15 F19:G19 F24:G24 F29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>168</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="13">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="14">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="15">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="15">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="15">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="16">
+        <v>17</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="8">
+        <v>14</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="16">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8">
+        <v>13</v>
+      </c>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="16">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="8">
+        <v>12</v>
+      </c>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="16">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="8">
+        <v>11</v>
+      </c>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="16">
+        <v>21</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="8">
+        <v>10</v>
+      </c>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="17">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="9">
+        <v>9</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="17">
+        <v>23</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="9">
+        <v>8</v>
+      </c>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="17">
+        <v>24</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="9">
+        <v>7</v>
+      </c>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17">
+        <v>25</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="9">
+        <v>6</v>
+      </c>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="17">
+        <v>26</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="9">
+        <v>5</v>
+      </c>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="19">
+        <v>27</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="20">
+        <v>4</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="19">
+        <v>28</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="20">
+        <v>3</v>
+      </c>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="19">
+        <v>29</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="20">
+        <v>2</v>
+      </c>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="19">
+        <v>30</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="20">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30">
-        <v>20</v>
-      </c>
-      <c r="D30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>